<commit_message>
added text file with filter values
</commit_message>
<xml_diff>
--- a/wiring.xlsx
+++ b/wiring.xlsx
@@ -149,8 +149,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -162,11 +174,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -184,8 +208,8 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>218729</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2829</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>187854</xdr:rowOff>
     </xdr:to>
@@ -661,20 +685,21 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L10" sqref="A1:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>